<commit_message>
added text to thesis
</commit_message>
<xml_diff>
--- a/figures/MCMC/Boxplot Table of values_95th.xlsx
+++ b/figures/MCMC/Boxplot Table of values_95th.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shakes/Dropbox/Apps/Overleaf/Thandolwethu Dlamini Thesis/templates/figures/MCMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A73D7718-9DD9-D045-9820-E9CDD08B9AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5378262-56F0-2E46-BE88-3EE3D6FD5198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{5C8FA220-1295-3F47-94E4-07B4D3FB7EAF}"/>
+    <workbookView xWindow="0" yWindow="19500" windowWidth="21600" windowHeight="18900" xr2:uid="{5C8FA220-1295-3F47-94E4-07B4D3FB7EAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,7 +81,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -121,7 +121,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A901DFE3-22FB-A540-815D-57F85F7600CE}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="F40" sqref="D40:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +457,7 @@
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -487,8 +487,12 @@
       <c r="E2" s="1">
         <v>17.653957999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" s="1">
+        <f>SUM(B2:E2)</f>
+        <v>101.224647</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -504,8 +508,9 @@
       <c r="E3" s="1">
         <v>13.646672000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -521,8 +526,9 @@
       <c r="E4" s="1">
         <v>5.0299999999999997E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -538,8 +544,12 @@
       <c r="E5" s="1">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="1">
+        <f t="shared" ref="G3:G9" si="0">SUM(B5:E5)</f>
+        <v>11.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -555,8 +565,9 @@
       <c r="E6" s="1">
         <v>6.8084730000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -572,8 +583,9 @@
       <c r="E7" s="1">
         <v>14.748761999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -589,8 +601,9 @@
       <c r="E8" s="1">
         <v>25.393574000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -606,8 +619,12 @@
       <c r="E9" s="1">
         <v>44.365000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>236.68800000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>